<commit_message>
Files are disappearing everywhere
</commit_message>
<xml_diff>
--- a/Business Audit/2022 Jul - 2023 Jun/Q4 Apr - Jun/Business Transaction Account Apr - Jun 2023.xlsx
+++ b/Business Audit/2022 Jul - 2023 Jun/Q4 Apr - Jun/Business Transaction Account Apr - Jun 2023.xlsx
@@ -741,9 +741,9 @@
       <c r="C4" s="7" t="n">
         <v>300</v>
       </c>
-      <c r="D4" s="7" t="n"/>
-      <c r="E4" s="7" t="n"/>
-      <c r="F4" s="7" t="n"/>
+      <c r="D4" s="7" t="inlineStr"/>
+      <c r="E4" s="7" t="inlineStr"/>
+      <c r="F4" s="7" t="inlineStr"/>
       <c r="G4" s="7">
         <f>SUM(C4:F4)</f>
         <v/>
@@ -16842,14 +16842,14 @@
       <c r="C4" s="7" t="n">
         <v>10</v>
       </c>
-      <c r="D4" s="7" t="n"/>
-      <c r="E4" s="7" t="n"/>
-      <c r="F4" s="7" t="n"/>
-      <c r="G4" s="7" t="n"/>
-      <c r="H4" s="7" t="n"/>
-      <c r="I4" s="7" t="n"/>
-      <c r="J4" s="7" t="n"/>
-      <c r="K4" s="7" t="n"/>
+      <c r="D4" s="7" t="inlineStr"/>
+      <c r="E4" s="7" t="inlineStr"/>
+      <c r="F4" s="7" t="inlineStr"/>
+      <c r="G4" s="7" t="inlineStr"/>
+      <c r="H4" s="7" t="inlineStr"/>
+      <c r="I4" s="7" t="inlineStr"/>
+      <c r="J4" s="7" t="inlineStr"/>
+      <c r="K4" s="7" t="inlineStr"/>
       <c r="L4" s="7">
         <f>SUM(C4:K4)</f>
         <v/>
@@ -16873,14 +16873,14 @@
       <c r="C5" s="7" t="n">
         <v>5000</v>
       </c>
-      <c r="D5" s="7" t="n"/>
-      <c r="E5" s="7" t="n"/>
-      <c r="F5" s="7" t="n"/>
-      <c r="G5" s="7" t="n"/>
-      <c r="H5" s="7" t="n"/>
-      <c r="I5" s="7" t="n"/>
-      <c r="J5" s="7" t="n"/>
-      <c r="K5" s="7" t="n"/>
+      <c r="D5" s="7" t="inlineStr"/>
+      <c r="E5" s="7" t="inlineStr"/>
+      <c r="F5" s="7" t="inlineStr"/>
+      <c r="G5" s="7" t="inlineStr"/>
+      <c r="H5" s="7" t="inlineStr"/>
+      <c r="I5" s="7" t="inlineStr"/>
+      <c r="J5" s="7" t="inlineStr"/>
+      <c r="K5" s="7" t="inlineStr"/>
       <c r="L5" s="7">
         <f>SUM(C5:K5)</f>
         <v/>
@@ -16904,14 +16904,14 @@
       <c r="C6" s="7" t="n">
         <v>10000</v>
       </c>
-      <c r="D6" s="7" t="n"/>
-      <c r="E6" s="7" t="n"/>
-      <c r="F6" s="7" t="n"/>
-      <c r="G6" s="7" t="n"/>
-      <c r="H6" s="7" t="n"/>
-      <c r="I6" s="7" t="n"/>
-      <c r="J6" s="7" t="n"/>
-      <c r="K6" s="7" t="n"/>
+      <c r="D6" s="7" t="inlineStr"/>
+      <c r="E6" s="7" t="inlineStr"/>
+      <c r="F6" s="7" t="inlineStr"/>
+      <c r="G6" s="7" t="inlineStr"/>
+      <c r="H6" s="7" t="inlineStr"/>
+      <c r="I6" s="7" t="inlineStr"/>
+      <c r="J6" s="7" t="inlineStr"/>
+      <c r="K6" s="7" t="inlineStr"/>
       <c r="L6" s="7">
         <f>SUM(C6:K6)</f>
         <v/>
@@ -16932,17 +16932,17 @@
           <t>Optus</t>
         </is>
       </c>
-      <c r="C7" s="7" t="n">
+      <c r="C7" s="7" t="inlineStr"/>
+      <c r="D7" s="7" t="inlineStr"/>
+      <c r="E7" s="7" t="inlineStr"/>
+      <c r="F7" s="7" t="inlineStr"/>
+      <c r="G7" s="7" t="inlineStr"/>
+      <c r="H7" s="7" t="inlineStr"/>
+      <c r="I7" s="7" t="inlineStr"/>
+      <c r="J7" s="7" t="inlineStr"/>
+      <c r="K7" s="7" t="n">
         <v>79</v>
       </c>
-      <c r="D7" s="7" t="n"/>
-      <c r="E7" s="7" t="n"/>
-      <c r="F7" s="7" t="n"/>
-      <c r="G7" s="7" t="n"/>
-      <c r="H7" s="7" t="n"/>
-      <c r="I7" s="7" t="n"/>
-      <c r="J7" s="7" t="n"/>
-      <c r="K7" s="7" t="n"/>
       <c r="L7" s="7">
         <f>SUM(C7:K7)</f>
         <v/>
@@ -16966,14 +16966,14 @@
       <c r="C8" s="7" t="n">
         <v>10</v>
       </c>
-      <c r="D8" s="7" t="n"/>
-      <c r="E8" s="7" t="n"/>
-      <c r="F8" s="7" t="n"/>
-      <c r="G8" s="7" t="n"/>
-      <c r="H8" s="7" t="n"/>
-      <c r="I8" s="7" t="n"/>
-      <c r="J8" s="7" t="n"/>
-      <c r="K8" s="7" t="n"/>
+      <c r="D8" s="7" t="inlineStr"/>
+      <c r="E8" s="7" t="inlineStr"/>
+      <c r="F8" s="7" t="inlineStr"/>
+      <c r="G8" s="7" t="inlineStr"/>
+      <c r="H8" s="7" t="inlineStr"/>
+      <c r="I8" s="7" t="inlineStr"/>
+      <c r="J8" s="7" t="inlineStr"/>
+      <c r="K8" s="7" t="inlineStr"/>
       <c r="L8" s="7">
         <f>SUM(C8:K8)</f>
         <v/>
@@ -16994,17 +16994,17 @@
           <t>Optus</t>
         </is>
       </c>
-      <c r="C9" s="7" t="n">
+      <c r="C9" s="7" t="inlineStr"/>
+      <c r="D9" s="7" t="inlineStr"/>
+      <c r="E9" s="7" t="inlineStr"/>
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="7" t="inlineStr"/>
+      <c r="H9" s="7" t="inlineStr"/>
+      <c r="I9" s="7" t="inlineStr"/>
+      <c r="J9" s="7" t="inlineStr"/>
+      <c r="K9" s="7" t="n">
         <v>79</v>
       </c>
-      <c r="D9" s="7" t="n"/>
-      <c r="E9" s="7" t="n"/>
-      <c r="F9" s="7" t="n"/>
-      <c r="G9" s="7" t="n"/>
-      <c r="H9" s="7" t="n"/>
-      <c r="I9" s="7" t="n"/>
-      <c r="J9" s="7" t="n"/>
-      <c r="K9" s="7" t="n"/>
       <c r="L9" s="7">
         <f>SUM(C9:K9)</f>
         <v/>
@@ -17028,14 +17028,14 @@
       <c r="C10" s="7" t="n">
         <v>300</v>
       </c>
-      <c r="D10" s="7" t="n"/>
-      <c r="E10" s="7" t="n"/>
-      <c r="F10" s="7" t="n"/>
-      <c r="G10" s="7" t="n"/>
-      <c r="H10" s="7" t="n"/>
-      <c r="I10" s="7" t="n"/>
-      <c r="J10" s="7" t="n"/>
-      <c r="K10" s="7" t="n"/>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="7" t="inlineStr"/>
+      <c r="G10" s="7" t="inlineStr"/>
+      <c r="H10" s="7" t="inlineStr"/>
+      <c r="I10" s="7" t="inlineStr"/>
+      <c r="J10" s="7" t="inlineStr"/>
+      <c r="K10" s="7" t="inlineStr"/>
       <c r="L10" s="7">
         <f>SUM(C10:K10)</f>
         <v/>
@@ -17056,17 +17056,17 @@
           <t>Transfer to xx9950 CommBank app Qi Qiong</t>
         </is>
       </c>
-      <c r="C11" s="7" t="n">
+      <c r="C11" s="7" t="inlineStr"/>
+      <c r="D11" s="7" t="inlineStr"/>
+      <c r="E11" s="7" t="n">
         <v>50</v>
       </c>
-      <c r="D11" s="7" t="n"/>
-      <c r="E11" s="7" t="n"/>
-      <c r="F11" s="7" t="n"/>
-      <c r="G11" s="7" t="n"/>
-      <c r="H11" s="7" t="n"/>
-      <c r="I11" s="7" t="n"/>
-      <c r="J11" s="7" t="n"/>
-      <c r="K11" s="7" t="n"/>
+      <c r="F11" s="7" t="inlineStr"/>
+      <c r="G11" s="7" t="inlineStr"/>
+      <c r="H11" s="7" t="inlineStr"/>
+      <c r="I11" s="7" t="inlineStr"/>
+      <c r="J11" s="7" t="inlineStr"/>
+      <c r="K11" s="7" t="inlineStr"/>
       <c r="L11" s="7">
         <f>SUM(C11:K11)</f>
         <v/>
@@ -17083,17 +17083,17 @@
           <t>Transfer to xx9950 CommBank app Qi Qiong</t>
         </is>
       </c>
-      <c r="C12" s="7" t="n">
+      <c r="C12" s="7" t="inlineStr"/>
+      <c r="D12" s="7" t="inlineStr"/>
+      <c r="E12" s="7" t="n">
         <v>50</v>
       </c>
-      <c r="D12" s="7" t="n"/>
-      <c r="E12" s="7" t="n"/>
-      <c r="F12" s="7" t="n"/>
-      <c r="G12" s="7" t="n"/>
-      <c r="H12" s="7" t="n"/>
-      <c r="I12" s="7" t="n"/>
-      <c r="J12" s="7" t="n"/>
-      <c r="K12" s="7" t="n"/>
+      <c r="F12" s="7" t="inlineStr"/>
+      <c r="G12" s="7" t="inlineStr"/>
+      <c r="H12" s="7" t="inlineStr"/>
+      <c r="I12" s="7" t="inlineStr"/>
+      <c r="J12" s="7" t="inlineStr"/>
+      <c r="K12" s="7" t="inlineStr"/>
       <c r="L12" s="7">
         <f>SUM(C12:K12)</f>
         <v/>
@@ -17110,17 +17110,17 @@
           <t>Transfer to xx9950 CommBank app Qi Qiong</t>
         </is>
       </c>
-      <c r="C13" s="7" t="n">
+      <c r="C13" s="7" t="inlineStr"/>
+      <c r="D13" s="7" t="inlineStr"/>
+      <c r="E13" s="7" t="n">
         <v>50</v>
       </c>
-      <c r="D13" s="7" t="n"/>
-      <c r="E13" s="7" t="n"/>
-      <c r="F13" s="7" t="n"/>
-      <c r="G13" s="7" t="n"/>
-      <c r="H13" s="7" t="n"/>
-      <c r="I13" s="7" t="n"/>
-      <c r="J13" s="7" t="n"/>
-      <c r="K13" s="7" t="n"/>
+      <c r="F13" s="7" t="inlineStr"/>
+      <c r="G13" s="7" t="inlineStr"/>
+      <c r="H13" s="7" t="inlineStr"/>
+      <c r="I13" s="7" t="inlineStr"/>
+      <c r="J13" s="7" t="inlineStr"/>
+      <c r="K13" s="7" t="inlineStr"/>
       <c r="L13" s="7">
         <f>SUM(C13:K13)</f>
         <v/>
@@ -17137,17 +17137,17 @@
           <t>Transfer to xx9950 CommBank app Qi Qiong</t>
         </is>
       </c>
-      <c r="C14" s="7" t="n">
+      <c r="C14" s="7" t="inlineStr"/>
+      <c r="D14" s="7" t="inlineStr"/>
+      <c r="E14" s="7" t="n">
         <v>7</v>
       </c>
-      <c r="D14" s="7" t="n"/>
-      <c r="E14" s="7" t="n"/>
-      <c r="F14" s="7" t="n"/>
-      <c r="G14" s="7" t="n"/>
-      <c r="H14" s="7" t="n"/>
-      <c r="I14" s="7" t="n"/>
-      <c r="J14" s="7" t="n"/>
-      <c r="K14" s="7" t="n"/>
+      <c r="F14" s="7" t="inlineStr"/>
+      <c r="G14" s="7" t="inlineStr"/>
+      <c r="H14" s="7" t="inlineStr"/>
+      <c r="I14" s="7" t="inlineStr"/>
+      <c r="J14" s="7" t="inlineStr"/>
+      <c r="K14" s="7" t="inlineStr"/>
       <c r="L14" s="7">
         <f>SUM(C14:K14)</f>
         <v/>
@@ -17164,17 +17164,17 @@
           <t>Transfer to xx9950 CommBank app Qi Qiong</t>
         </is>
       </c>
-      <c r="C15" s="7" t="n">
+      <c r="C15" s="7" t="inlineStr"/>
+      <c r="D15" s="7" t="inlineStr"/>
+      <c r="E15" s="7" t="n">
         <v>20</v>
       </c>
-      <c r="D15" s="7" t="n"/>
-      <c r="E15" s="7" t="n"/>
-      <c r="F15" s="7" t="n"/>
-      <c r="G15" s="7" t="n"/>
-      <c r="H15" s="7" t="n"/>
-      <c r="I15" s="7" t="n"/>
-      <c r="J15" s="7" t="n"/>
-      <c r="K15" s="7" t="n"/>
+      <c r="F15" s="7" t="inlineStr"/>
+      <c r="G15" s="7" t="inlineStr"/>
+      <c r="H15" s="7" t="inlineStr"/>
+      <c r="I15" s="7" t="inlineStr"/>
+      <c r="J15" s="7" t="inlineStr"/>
+      <c r="K15" s="7" t="inlineStr"/>
       <c r="L15" s="7">
         <f>SUM(C15:K15)</f>
         <v/>
@@ -17191,17 +17191,17 @@
           <t>Transfer to xx9950 CommBank app Qi Qiong</t>
         </is>
       </c>
-      <c r="C16" s="7" t="n">
+      <c r="C16" s="7" t="inlineStr"/>
+      <c r="D16" s="7" t="inlineStr"/>
+      <c r="E16" s="7" t="n">
         <v>50</v>
       </c>
-      <c r="D16" s="7" t="n"/>
-      <c r="E16" s="7" t="n"/>
-      <c r="F16" s="7" t="n"/>
-      <c r="G16" s="7" t="n"/>
-      <c r="H16" s="7" t="n"/>
-      <c r="I16" s="7" t="n"/>
-      <c r="J16" s="7" t="n"/>
-      <c r="K16" s="7" t="n"/>
+      <c r="F16" s="7" t="inlineStr"/>
+      <c r="G16" s="7" t="inlineStr"/>
+      <c r="H16" s="7" t="inlineStr"/>
+      <c r="I16" s="7" t="inlineStr"/>
+      <c r="J16" s="7" t="inlineStr"/>
+      <c r="K16" s="7" t="inlineStr"/>
       <c r="L16" s="7">
         <f>SUM(C16:K16)</f>
         <v/>
@@ -17218,17 +17218,17 @@
           <t>Transfer to xx9950 CommBank app Qi Qiong</t>
         </is>
       </c>
-      <c r="C17" s="7" t="n">
+      <c r="C17" s="7" t="inlineStr"/>
+      <c r="D17" s="7" t="inlineStr"/>
+      <c r="E17" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D17" s="7" t="n"/>
-      <c r="E17" s="7" t="n"/>
-      <c r="F17" s="7" t="n"/>
-      <c r="G17" s="7" t="n"/>
-      <c r="H17" s="7" t="n"/>
-      <c r="I17" s="7" t="n"/>
-      <c r="J17" s="7" t="n"/>
-      <c r="K17" s="7" t="n"/>
+      <c r="F17" s="7" t="inlineStr"/>
+      <c r="G17" s="7" t="inlineStr"/>
+      <c r="H17" s="7" t="inlineStr"/>
+      <c r="I17" s="7" t="inlineStr"/>
+      <c r="J17" s="7" t="inlineStr"/>
+      <c r="K17" s="7" t="inlineStr"/>
       <c r="L17" s="7">
         <f>SUM(C17:K17)</f>
         <v/>
@@ -17249,17 +17249,17 @@
           <t>Transfer to xx9950 CommBank app Qi Qiong</t>
         </is>
       </c>
-      <c r="C18" s="7" t="n">
+      <c r="C18" s="7" t="inlineStr"/>
+      <c r="D18" s="7" t="inlineStr"/>
+      <c r="E18" s="7" t="n">
         <v>40</v>
       </c>
-      <c r="D18" s="7" t="n"/>
-      <c r="E18" s="7" t="n"/>
-      <c r="F18" s="7" t="n"/>
-      <c r="G18" s="7" t="n"/>
-      <c r="H18" s="7" t="n"/>
-      <c r="I18" s="7" t="n"/>
-      <c r="J18" s="7" t="n"/>
-      <c r="K18" s="7" t="n"/>
+      <c r="F18" s="7" t="inlineStr"/>
+      <c r="G18" s="7" t="inlineStr"/>
+      <c r="H18" s="7" t="inlineStr"/>
+      <c r="I18" s="7" t="inlineStr"/>
+      <c r="J18" s="7" t="inlineStr"/>
+      <c r="K18" s="7" t="inlineStr"/>
       <c r="L18" s="7">
         <f>SUM(C18:K18)</f>
         <v/>
@@ -17283,14 +17283,14 @@
       <c r="C19" s="7" t="n">
         <v>10</v>
       </c>
-      <c r="D19" s="7" t="n"/>
-      <c r="E19" s="7" t="n"/>
-      <c r="F19" s="7" t="n"/>
-      <c r="G19" s="7" t="n"/>
-      <c r="H19" s="7" t="n"/>
-      <c r="I19" s="7" t="n"/>
-      <c r="J19" s="7" t="n"/>
-      <c r="K19" s="7" t="n"/>
+      <c r="D19" s="7" t="inlineStr"/>
+      <c r="E19" s="7" t="inlineStr"/>
+      <c r="F19" s="7" t="inlineStr"/>
+      <c r="G19" s="7" t="inlineStr"/>
+      <c r="H19" s="7" t="inlineStr"/>
+      <c r="I19" s="7" t="inlineStr"/>
+      <c r="J19" s="7" t="inlineStr"/>
+      <c r="K19" s="7" t="inlineStr"/>
       <c r="L19" s="7">
         <f>SUM(C19:K19)</f>
         <v/>
@@ -17311,17 +17311,17 @@
           <t>Transfer to xx9950 CommBank app Qi Qiong</t>
         </is>
       </c>
-      <c r="C20" s="7" t="n">
+      <c r="C20" s="7" t="inlineStr"/>
+      <c r="D20" s="7" t="inlineStr"/>
+      <c r="E20" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D20" s="7" t="n"/>
-      <c r="E20" s="7" t="n"/>
-      <c r="F20" s="7" t="n"/>
-      <c r="G20" s="7" t="n"/>
-      <c r="H20" s="7" t="n"/>
-      <c r="I20" s="7" t="n"/>
-      <c r="J20" s="7" t="n"/>
-      <c r="K20" s="7" t="n"/>
+      <c r="F20" s="7" t="inlineStr"/>
+      <c r="G20" s="7" t="inlineStr"/>
+      <c r="H20" s="7" t="inlineStr"/>
+      <c r="I20" s="7" t="inlineStr"/>
+      <c r="J20" s="7" t="inlineStr"/>
+      <c r="K20" s="7" t="inlineStr"/>
       <c r="L20" s="7">
         <f>SUM(C20:K20)</f>
         <v/>
@@ -17342,17 +17342,17 @@
           <t>Optus</t>
         </is>
       </c>
-      <c r="C21" s="7" t="n">
+      <c r="C21" s="7" t="inlineStr"/>
+      <c r="D21" s="7" t="inlineStr"/>
+      <c r="E21" s="7" t="inlineStr"/>
+      <c r="F21" s="7" t="inlineStr"/>
+      <c r="G21" s="7" t="inlineStr"/>
+      <c r="H21" s="7" t="inlineStr"/>
+      <c r="I21" s="7" t="inlineStr"/>
+      <c r="J21" s="7" t="inlineStr"/>
+      <c r="K21" s="7" t="n">
         <v>79</v>
       </c>
-      <c r="D21" s="7" t="n"/>
-      <c r="E21" s="7" t="n"/>
-      <c r="F21" s="7" t="n"/>
-      <c r="G21" s="7" t="n"/>
-      <c r="H21" s="7" t="n"/>
-      <c r="I21" s="7" t="n"/>
-      <c r="J21" s="7" t="n"/>
-      <c r="K21" s="7" t="n"/>
       <c r="L21" s="7">
         <f>SUM(C21:K21)</f>
         <v/>

</xml_diff>